<commit_message>
REPORT & cloture job
fix comm_Q, new report, adresse client, cloture job
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/Report LoS.xlsx
+++ b/lib/PHPExcel/templates/Report LoS.xlsx
@@ -849,15 +849,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -890,9 +881,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1009,6 +997,18 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1441,7 +1441,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="64" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="1"/>
@@ -1455,7 +1455,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="64" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="1"/>
@@ -1500,20 +1500,20 @@
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
       <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1526,20 +1526,20 @@
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
       <c r="H9" s="10" t="s">
         <v>9</v>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="67" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="7"/>
@@ -1569,16 +1569,16 @@
       <c r="B13" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="65"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="65"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="69"/>
+      <c r="C15" s="65"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
@@ -1607,18 +1607,18 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="95" t="s">
+      <c r="K19" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="L19" s="95" t="s">
+      <c r="L19" s="91" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="89" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1697,16 +1697,16 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="70"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="71"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="67"/>
       <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +1815,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="92" t="s">
+      <c r="A51" s="88" t="s">
         <v>87</v>
       </c>
       <c r="H51" s="27"/>
@@ -1882,7 +1882,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12:XFD14"/>
+      <selection pane="topRight" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1906,7 +1906,7 @@
       <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
@@ -1916,7 +1916,7 @@
       <c r="C6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="46"/>
     </row>
     <row r="7" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
@@ -1926,7 +1926,7 @@
       <c r="C7" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="50"/>
+      <c r="D7" s="47"/>
     </row>
     <row r="8" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
@@ -1936,7 +1936,7 @@
       <c r="C8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="50"/>
+      <c r="D8" s="47"/>
     </row>
     <row r="9" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
@@ -1946,7 +1946,7 @@
       <c r="C9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="47"/>
     </row>
     <row r="10" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="36"/>
-      <c r="D10" s="94"/>
+      <c r="D10" s="90"/>
     </row>
     <row r="11" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
@@ -1964,7 +1964,7 @@
       <c r="C11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
@@ -1974,7 +1974,7 @@
       <c r="C12" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="47"/>
     </row>
     <row r="13" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
@@ -1984,37 +1984,37 @@
       <c r="C13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="50"/>
+      <c r="D13" s="47"/>
     </row>
     <row r="14" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="81"/>
-      <c r="B14" s="82" t="s">
+      <c r="A14" s="77"/>
+      <c r="B14" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="99"/>
+      <c r="C14" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="95"/>
     </row>
     <row r="15" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
-      <c r="B15" s="85" t="s">
+      <c r="A15" s="80"/>
+      <c r="B15" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="96"/>
     </row>
     <row r="16" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="61"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="57"/>
     </row>
     <row r="17" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
@@ -2024,7 +2024,7 @@
       <c r="C17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="90"/>
+      <c r="D17" s="86"/>
     </row>
     <row r="18" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
@@ -2034,55 +2034,55 @@
       <c r="C18" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="90"/>
+      <c r="D18" s="86"/>
     </row>
     <row r="19" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="60" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="91"/>
+      <c r="D19" s="87"/>
     </row>
     <row r="20" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="61"/>
+      <c r="D20" s="57"/>
     </row>
     <row r="21" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="62" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="50"/>
     </row>
     <row r="22" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="62" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="39"/>
       <c r="C22" s="37"/>
-      <c r="D22" s="53"/>
+      <c r="D22" s="50"/>
     </row>
     <row r="23" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="62" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="50"/>
     </row>
     <row r="24" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
@@ -2092,86 +2092,86 @@
       <c r="C24" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="52"/>
+      <c r="D24" s="49"/>
     </row>
     <row r="25" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="39"/>
       <c r="C25" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="76" t="s">
+      <c r="B26" s="71"/>
+      <c r="C26" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="77"/>
+      <c r="D26" s="73"/>
     </row>
     <row r="27" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="94"/>
     </row>
     <row r="28" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="68" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="53"/>
+      <c r="D28" s="50"/>
     </row>
     <row r="29" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="68" t="s">
         <v>94</v>
       </c>
       <c r="C29" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="53"/>
+      <c r="D29" s="50"/>
     </row>
     <row r="30" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="69" t="s">
         <v>95</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="62"/>
+      <c r="D30" s="58"/>
     </row>
     <row r="31" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="61"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
     </row>
     <row r="32" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="41" t="s">
@@ -2180,10 +2180,10 @@
       <c r="C32" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="53"/>
+      <c r="D32" s="50"/>
     </row>
     <row r="33" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="39" t="s">
@@ -2192,10 +2192,10 @@
       <c r="C33" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="53"/>
+      <c r="D33" s="50"/>
     </row>
     <row r="34" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="39" t="s">
@@ -2204,7 +2204,7 @@
       <c r="C34" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="53"/>
+      <c r="D34" s="50"/>
     </row>
     <row r="35" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
@@ -2216,10 +2216,10 @@
       <c r="C35" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="52"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="62" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="39" t="s">
@@ -2228,10 +2228,10 @@
       <c r="C36" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="54"/>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="62" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="39" t="s">
@@ -2240,10 +2240,10 @@
       <c r="C37" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="55"/>
+      <c r="D37" s="52"/>
     </row>
     <row r="38" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="62" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="39" t="s">
@@ -2252,10 +2252,10 @@
       <c r="C38" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="55"/>
+      <c r="D38" s="52"/>
     </row>
     <row r="39" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="62" t="s">
         <v>24</v>
       </c>
       <c r="B39" s="39" t="s">
@@ -2264,10 +2264,10 @@
       <c r="C39" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="55"/>
+      <c r="D39" s="52"/>
     </row>
     <row r="40" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="63" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="40" t="s">
@@ -2276,15 +2276,15 @@
       <c r="C40" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="63"/>
+      <c r="D40" s="59"/>
     </row>
     <row r="41" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="59"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="35"/>
-      <c r="D41" s="61"/>
+      <c r="D41" s="57"/>
     </row>
     <row r="42" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="B42" s="34"/>
       <c r="C42" s="36"/>
-      <c r="D42" s="50"/>
+      <c r="D42" s="47"/>
     </row>
     <row r="43" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="B43" s="34"/>
       <c r="C43" s="36"/>
-      <c r="D43" s="50"/>
+      <c r="D43" s="47"/>
     </row>
     <row r="44" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
@@ -2310,7 +2310,7 @@
       <c r="C44" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="50"/>
+      <c r="D44" s="47"/>
     </row>
     <row r="45" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
@@ -2320,7 +2320,7 @@
       <c r="C45" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="50"/>
+      <c r="D45" s="47"/>
     </row>
     <row r="46" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
@@ -2330,7 +2330,7 @@
       <c r="C46" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="51"/>
+      <c r="D46" s="48"/>
     </row>
     <row r="47" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="42" t="s">
@@ -2340,128 +2340,128 @@
       <c r="C47" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="96"/>
-    </row>
-    <row r="48" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="58"/>
+      <c r="D47" s="92"/>
+    </row>
+    <row r="48" spans="1:4" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="98"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="101"/>
     </row>
     <row r="49" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="46"/>
-      <c r="D49" s="47"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="44"/>
     </row>
     <row r="50" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="57"/>
-      <c r="P50" s="57"/>
-      <c r="Q50" s="57"/>
-      <c r="R50" s="57"/>
-      <c r="S50" s="57"/>
-      <c r="T50" s="57"/>
-      <c r="U50" s="57"/>
-      <c r="V50" s="57"/>
-      <c r="W50" s="57"/>
-      <c r="X50" s="57"/>
-      <c r="Y50" s="57"/>
-      <c r="Z50" s="57"/>
-      <c r="AA50" s="57"/>
-      <c r="AB50" s="57"/>
-      <c r="AC50" s="57"/>
-      <c r="AD50" s="57"/>
-      <c r="AE50" s="57"/>
-      <c r="AF50" s="57"/>
-      <c r="AG50" s="57"/>
-      <c r="AH50" s="57"/>
-      <c r="AI50" s="57"/>
-      <c r="AJ50" s="57"/>
-      <c r="AK50" s="57"/>
-      <c r="AL50" s="57"/>
-      <c r="AM50" s="57"/>
-      <c r="AN50" s="57"/>
-      <c r="AO50" s="57"/>
-      <c r="AP50" s="57"/>
-      <c r="AQ50" s="57"/>
-      <c r="AR50" s="57"/>
-      <c r="AS50" s="57"/>
-      <c r="AT50" s="57"/>
-      <c r="AU50" s="57"/>
-      <c r="AV50" s="57"/>
-      <c r="AW50" s="57"/>
-      <c r="AX50" s="57"/>
-      <c r="AY50" s="57"/>
-      <c r="AZ50" s="57"/>
-      <c r="BA50" s="57"/>
-      <c r="BB50" s="57"/>
-      <c r="BC50" s="57"/>
-      <c r="BD50" s="57"/>
-      <c r="BE50" s="57"/>
-      <c r="BF50" s="57"/>
-      <c r="BG50" s="57"/>
-      <c r="BH50" s="57"/>
-      <c r="BI50" s="57"/>
-      <c r="BJ50" s="57"/>
-      <c r="BK50" s="57"/>
-      <c r="BL50" s="57"/>
-      <c r="BM50" s="57"/>
-      <c r="BN50" s="57"/>
-      <c r="BO50" s="57"/>
-      <c r="BP50" s="57"/>
-      <c r="BQ50" s="57"/>
-      <c r="BR50" s="57"/>
-      <c r="BS50" s="57"/>
-      <c r="BT50" s="57"/>
-      <c r="BU50" s="57"/>
-      <c r="BV50" s="57"/>
-      <c r="BW50" s="57"/>
-      <c r="BX50" s="57"/>
-      <c r="BY50" s="57"/>
-      <c r="BZ50" s="57"/>
-      <c r="CA50" s="57"/>
-      <c r="CB50" s="57"/>
-      <c r="CC50" s="57"/>
-      <c r="CD50" s="57"/>
-      <c r="CE50" s="57"/>
-      <c r="CF50" s="57"/>
-      <c r="CG50" s="57"/>
-      <c r="CH50" s="57"/>
-      <c r="CI50" s="57"/>
-      <c r="CJ50" s="57"/>
-      <c r="CK50" s="57"/>
-      <c r="CL50" s="57"/>
-      <c r="CM50" s="57"/>
-      <c r="CN50" s="57"/>
-      <c r="CO50" s="57"/>
-      <c r="CP50" s="57"/>
-      <c r="CQ50" s="57"/>
-      <c r="CR50" s="57"/>
-      <c r="CS50" s="57"/>
-      <c r="CT50" s="57"/>
-      <c r="CU50" s="57"/>
-      <c r="CV50" s="57"/>
-      <c r="CW50" s="57"/>
-      <c r="CX50" s="57"/>
-      <c r="CY50" s="57"/>
+      <c r="C50" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
+      <c r="K50" s="54"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="54"/>
+      <c r="N50" s="54"/>
+      <c r="O50" s="54"/>
+      <c r="P50" s="54"/>
+      <c r="Q50" s="54"/>
+      <c r="R50" s="54"/>
+      <c r="S50" s="54"/>
+      <c r="T50" s="54"/>
+      <c r="U50" s="54"/>
+      <c r="V50" s="54"/>
+      <c r="W50" s="54"/>
+      <c r="X50" s="54"/>
+      <c r="Y50" s="54"/>
+      <c r="Z50" s="54"/>
+      <c r="AA50" s="54"/>
+      <c r="AB50" s="54"/>
+      <c r="AC50" s="54"/>
+      <c r="AD50" s="54"/>
+      <c r="AE50" s="54"/>
+      <c r="AF50" s="54"/>
+      <c r="AG50" s="54"/>
+      <c r="AH50" s="54"/>
+      <c r="AI50" s="54"/>
+      <c r="AJ50" s="54"/>
+      <c r="AK50" s="54"/>
+      <c r="AL50" s="54"/>
+      <c r="AM50" s="54"/>
+      <c r="AN50" s="54"/>
+      <c r="AO50" s="54"/>
+      <c r="AP50" s="54"/>
+      <c r="AQ50" s="54"/>
+      <c r="AR50" s="54"/>
+      <c r="AS50" s="54"/>
+      <c r="AT50" s="54"/>
+      <c r="AU50" s="54"/>
+      <c r="AV50" s="54"/>
+      <c r="AW50" s="54"/>
+      <c r="AX50" s="54"/>
+      <c r="AY50" s="54"/>
+      <c r="AZ50" s="54"/>
+      <c r="BA50" s="54"/>
+      <c r="BB50" s="54"/>
+      <c r="BC50" s="54"/>
+      <c r="BD50" s="54"/>
+      <c r="BE50" s="54"/>
+      <c r="BF50" s="54"/>
+      <c r="BG50" s="54"/>
+      <c r="BH50" s="54"/>
+      <c r="BI50" s="54"/>
+      <c r="BJ50" s="54"/>
+      <c r="BK50" s="54"/>
+      <c r="BL50" s="54"/>
+      <c r="BM50" s="54"/>
+      <c r="BN50" s="54"/>
+      <c r="BO50" s="54"/>
+      <c r="BP50" s="54"/>
+      <c r="BQ50" s="54"/>
+      <c r="BR50" s="54"/>
+      <c r="BS50" s="54"/>
+      <c r="BT50" s="54"/>
+      <c r="BU50" s="54"/>
+      <c r="BV50" s="54"/>
+      <c r="BW50" s="54"/>
+      <c r="BX50" s="54"/>
+      <c r="BY50" s="54"/>
+      <c r="BZ50" s="54"/>
+      <c r="CA50" s="54"/>
+      <c r="CB50" s="54"/>
+      <c r="CC50" s="54"/>
+      <c r="CD50" s="54"/>
+      <c r="CE50" s="54"/>
+      <c r="CF50" s="54"/>
+      <c r="CG50" s="54"/>
+      <c r="CH50" s="54"/>
+      <c r="CI50" s="54"/>
+      <c r="CJ50" s="54"/>
+      <c r="CK50" s="54"/>
+      <c r="CL50" s="54"/>
+      <c r="CM50" s="54"/>
+      <c r="CN50" s="54"/>
+      <c r="CO50" s="54"/>
+      <c r="CP50" s="54"/>
+      <c r="CQ50" s="54"/>
+      <c r="CR50" s="54"/>
+      <c r="CS50" s="54"/>
+      <c r="CT50" s="54"/>
+      <c r="CU50" s="54"/>
+      <c r="CV50" s="54"/>
+      <c r="CW50" s="54"/>
+      <c r="CX50" s="54"/>
+      <c r="CY50" s="54"/>
     </row>
     <row r="51" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="46"/>
+      <c r="C51" s="43"/>
     </row>
     <row r="52" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="29" t="s">
@@ -2470,19 +2470,19 @@
       <c r="C52" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="48"/>
+      <c r="D52" s="45"/>
     </row>
     <row r="53" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="47"/>
+      <c r="D53" s="44"/>
     </row>
     <row r="54" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="48"/>
+      <c r="D54" s="45"/>
     </row>
     <row r="55" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="47"/>
+      <c r="D55" s="44"/>
     </row>
     <row r="56" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="48"/>
+      <c r="D56" s="45"/>
     </row>
     <row r="74" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -2514,14 +2514,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="89"/>
-      <c r="D1" s="97" t="s">
+      <c r="A1" s="85"/>
+      <c r="D1" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="87"/>
+      <c r="G1" s="83"/>
       <c r="H1" s="21">
         <f>+'En-tête'!J5</f>
         <v>0</v>
@@ -2546,29 +2546,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Check xmlns="67604082-326d-4240-aaee-100283b20839">Rapport Validé</Check>
-    <vctj xmlns="67604082-326d-4240-aaee-100283b20839">8043</vctj>
-    <pv7j xmlns="67604082-326d-4240-aaee-100283b20839">13232</pv7j>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006A18800F7AB66843AE086E8500CCEA21" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d60d5c9f17a480d7e4b53ebba2c4603">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67604082-326d-4240-aaee-100283b20839" xmlns:ns3="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b97804bffc58ba73e5228c2548755f2" ns2:_="" ns3:_="">
     <xsd:import namespace="67604082-326d-4240-aaee-100283b20839"/>
@@ -2744,40 +2721,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07ED7936-D779-47E7-BF6C-7C086F04E976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="67604082-326d-4240-aaee-100283b20839"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C53B3C-BBC9-48C3-9DA4-3687FEE00EE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39F1329F-71F7-4F0E-A822-5837ADF5B51C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Check xmlns="67604082-326d-4240-aaee-100283b20839">Rapport Validé</Check>
+    <vctj xmlns="67604082-326d-4240-aaee-100283b20839">8043</vctj>
+    <pv7j xmlns="67604082-326d-4240-aaee-100283b20839">13232</pv7j>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{386C40D6-9904-47D7-9FC5-798E8189EC7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2794,4 +2761,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39F1329F-71F7-4F0E-A822-5837ADF5B51C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C53B3C-BBC9-48C3-9DA4-3687FEE00EE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07ED7936-D779-47E7-BF6C-7C086F04E976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="67604082-326d-4240-aaee-100283b20839"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>